<commit_message>
update docs and tests
</commit_message>
<xml_diff>
--- a/documents/Гранч/tests.xlsx
+++ b/documents/Гранч/tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git repositories\HypernetTest\documents\тесты\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git repositories\HypernetTest\documents\Гранч\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2340F6-F505-4F5C-8944-3E7E6C65E800}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA0FF5A-E0A8-453E-BA3C-AF2600674EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
@@ -353,8 +353,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -638,270 +644,282 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G12"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>14</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>28</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>13</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>42</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>14</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>56</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>16</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>14</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>28</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>13</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>14</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>42</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>12</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>14</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>56</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>17</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>28</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>42</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>15</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>28</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>56</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>17</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>17</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>42</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>56</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>16</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>16</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -910,144 +928,154 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB023486-AA0A-4DFE-AAE8-59573CFDF263}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1056,144 +1084,164 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A73072CE-7B4E-4B6C-B281-4B09DA1F9546}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>